<commit_message>
General Info updated #38
typo removed and changed likelihood -> log-likelihood
</commit_message>
<xml_diff>
--- a/hackathon_contributions_new_data_format/Swameye_PNAS2003/General_info.xlsx
+++ b/hackathon_contributions_new_data_format/Swameye_PNAS2003/General_info.xlsx
@@ -34,13 +34,13 @@
     <t xml:space="preserve">FACTS</t>
   </si>
   <si>
-    <t xml:space="preserve">The model contains 46 data points, 16 free parameters and 1 experimental conditions</t>
+    <t xml:space="preserve">The model contains 46 data points, 13 free parameters and 1 experimental conditions</t>
   </si>
   <si>
     <t xml:space="preserve">Errors are assumed as additive Gaussian errors</t>
   </si>
   <si>
-    <t xml:space="preserve">Likelihood value of the model is </t>
+    <t xml:space="preserve">Log-likelihood value of the model is </t>
   </si>
   <si>
     <t xml:space="preserve">Chi2 value of the model is </t>
@@ -443,8 +443,8 @@
   </sheetPr>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -563,7 +563,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -584,8 +584,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -891,7 +890,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -906,8 +905,8 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1072,7 +1071,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1088,14 +1087,12 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,7 +1259,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>